<commit_message>
DOE PI poster updates
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
+++ b/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA21290-2D21-4A5D-B0E2-F5CDEA4B0EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B11AD-EEF6-4A15-852E-70B0FA0F75B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2175" yWindow="1020" windowWidth="21600" windowHeight="11295" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
+    <workbookView xWindow="-23148" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Point</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Center channel piezometer 1</t>
   </si>
   <si>
-    <t>Actual piezometer</t>
-  </si>
-  <si>
     <t>Center channel T stake 1</t>
   </si>
   <si>
@@ -88,12 +85,6 @@
     <t>Base to step</t>
   </si>
   <si>
-    <t>Piezometers z</t>
-  </si>
-  <si>
-    <t>1m.</t>
-  </si>
-  <si>
     <t>Center of river o piezo 2</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>Top of rock</t>
   </si>
   <si>
-    <t>T probe</t>
-  </si>
-  <si>
     <t>Center of river T probe</t>
   </si>
   <si>
@@ -142,9 +130,6 @@
     <t>End of antenna</t>
   </si>
   <si>
-    <t>Piezometer necst</t>
-  </si>
-  <si>
     <t>(dry)</t>
   </si>
   <si>
@@ -163,9 +148,6 @@
     <t>Hydrophone pipe top</t>
   </si>
   <si>
-    <t>T probe 3</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -203,6 +185,24 @@
   </si>
   <si>
     <t>Instrument (HI)</t>
+  </si>
+  <si>
+    <t>Actual piezometer (bottom)</t>
+  </si>
+  <si>
+    <t>LANL</t>
+  </si>
+  <si>
+    <t>Piezometer nest 2</t>
+  </si>
+  <si>
+    <t>Piezometer nest 3</t>
+  </si>
+  <si>
+    <t>T probe 8</t>
+  </si>
+  <si>
+    <t>T probe 2</t>
   </si>
 </sst>
 </file>
@@ -252,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -383,11 +383,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -417,8 +441,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,14 +453,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,6 +466,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -456,9 +496,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,6 +513,1507 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Downstream Reach Thalweg</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.55347324270619758"/>
+                  <c:y val="0.17602833651625102"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="94"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29999999999999716</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>22.715000000000003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>25.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>27.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>33.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>35.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>35.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>36.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>36.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>37.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>39.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>41.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="94"/>
+                <c:pt idx="0">
+                  <c:v>2721.752</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2721.752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2721.7419999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2721.7559999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2721.7619999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2721.732</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2721.732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2721.7619999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2721.7819999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2721.8069999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2721.8819999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2721.962</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2721.962</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2722.0119999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2722.047</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2722.0619999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2722.0969999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2722.1519999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2722.1319999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2722.1419999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2722.2169999999996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2722.1819999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2722.2169999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2722.2919999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2722.3419999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2722.4319999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2722.4919999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2722.4719999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2722.4869999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2722.5719999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2722.6169999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2722.587</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2722.587</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2722.5519999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2722.5789999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2722.5619999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2722.6519999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2722.6539999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2722.7789999999995</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2722.6989999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2723.0039999999995</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2723.0239999999994</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2723.0789999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2723.0739999999996</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2723.0039999999995</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2723.0989999999997</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2723.0489999999995</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2723.1789999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2723.1889999999994</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2723.1889999999994</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2723.1689999999994</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2723.1589999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2723.1489999999994</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2723.1589999999997</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2723.2389999999996</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2723.2589999999996</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2723.5189999999993</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2723.4289999999996</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2723.4489999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2723.4069999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2723.5189999999993</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2723.6589999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2723.5789999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2723.7089999999994</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2723.6689999999994</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2723.7089999999994</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2723.8189999999995</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2723.8389999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2723.8389999999995</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2723.8789999999995</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2723.9239999999995</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2723.8839999999996</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2724.0789999999993</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2724.1639999999993</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2724.1839999999993</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2724.2139999999995</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2724.1939999999995</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2724.2289999999994</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2724.5539999999992</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2724.6239999999993</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2724.5539999999992</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2724.5839999999994</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2724.5539999999992</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2724.5739999999996</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2724.6039999999994</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2724.6389999999992</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2724.6589999999992</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2724.6439999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2724.6589999999992</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2724.7439999999992</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2724.7489999999993</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2724.7439999999992</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2724.7139999999995</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2724.7439999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4807-44C4-ACE0-DE8BD0294A45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1853070912"/>
+        <c:axId val="1853073408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1853070912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853073408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1853073408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1853070912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285748</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>280146</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEAB62E-190B-CD5B-E908-5B0A74536C9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,10 +2313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64046064-0207-40E0-86BF-2B34A938C764}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,15 +2331,15 @@
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="F1" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -815,20 +2353,20 @@
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="23"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -837,18 +2375,18 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>15</v>
+      <c r="G3" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -857,16 +2395,19 @@
         <v>2.16</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="24">
+        <f>I5-C4</f>
+        <v>2721.752</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>32.5</v>
       </c>
@@ -874,17 +2415,23 @@
       <c r="C5" s="10">
         <v>2.16</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="10">
+      <c r="D5" s="12"/>
+      <c r="E5" s="25">
+        <v>2721.752</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="22">
+        <f>E5+C5</f>
+        <v>2723.9119999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>32.799999999999997</v>
       </c>
@@ -893,15 +2440,18 @@
         <v>2.17</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="25"/>
+      <c r="E6" s="9">
+        <f>$I$5-C6</f>
+        <v>2721.7419999999997</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="10">
         <f>A6-32.5</f>
         <v>0.29999999999999716</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>33.5</v>
       </c>
@@ -910,17 +2460,20 @@
         <v>2.1560000000000001</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="25"/>
+      <c r="E7" s="10">
+        <f t="shared" ref="E7:E29" si="0">$I$5-C7</f>
+        <v>2721.7559999999999</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="29"/>
       <c r="H7" s="10">
-        <f t="shared" ref="H7:H70" si="0">A7-32.5</f>
+        <f t="shared" ref="H7:H70" si="1">A7-32.5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>33.5</v>
       </c>
@@ -929,17 +2482,26 @@
         <v>2.15</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="25"/>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.7619999999997</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="29"/>
       <c r="H8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="26">
+        <v>2721.848</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>34</v>
       </c>
@@ -948,15 +2510,18 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="25"/>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.732</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>34.5</v>
       </c>
@@ -965,15 +2530,18 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="25"/>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.732</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>35</v>
       </c>
@@ -982,15 +2550,18 @@
         <v>2.15</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.7619999999997</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>35.6</v>
       </c>
@@ -999,17 +2570,20 @@
         <v>2.13</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="25"/>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.7819999999997</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="29"/>
       <c r="H12" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1000000000000014</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>36</v>
       </c>
@@ -1018,15 +2592,18 @@
         <v>2.105</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="25"/>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.8069999999998</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>36.6</v>
       </c>
@@ -1035,15 +2612,18 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="25"/>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.8819999999996</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1000000000000014</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>37</v>
       </c>
@@ -1052,15 +2632,18 @@
         <v>1.95</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="25"/>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.962</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>37.5</v>
       </c>
@@ -1069,11 +2652,14 @@
         <v>1.95</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="25"/>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>2721.962</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -1086,11 +2672,14 @@
         <v>1.9</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="25"/>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.0119999999997</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
     </row>
@@ -1103,11 +2692,14 @@
         <v>1.865</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.047</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1120,11 +2712,14 @@
         <v>1.85</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="25"/>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.0619999999999</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="29"/>
       <c r="H19" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
     </row>
@@ -1137,11 +2732,14 @@
         <v>1.8149999999999999</v>
       </c>
       <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="25"/>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.0969999999998</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1154,11 +2752,14 @@
         <v>1.76</v>
       </c>
       <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="25"/>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.1519999999996</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
     </row>
@@ -1171,11 +2772,14 @@
         <v>1.78</v>
       </c>
       <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="25"/>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.1319999999996</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1188,13 +2792,16 @@
         <v>1.77</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G23" s="25"/>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.1419999999998</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="29"/>
       <c r="H23" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
@@ -1207,11 +2814,14 @@
         <v>1.6950000000000001</v>
       </c>
       <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="25"/>
+      <c r="E24" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.2169999999996</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="29"/>
       <c r="H24" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -1224,11 +2834,14 @@
         <v>1.73</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="25"/>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.1819999999998</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
     </row>
@@ -1241,11 +2854,14 @@
         <v>1.6950000000000001</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="25"/>
+      <c r="E26" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.2169999999996</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -1258,13 +2874,16 @@
         <v>1.62</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="25"/>
+      <c r="E27" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.2919999999999</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="29"/>
       <c r="H27" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.700000000000003</v>
       </c>
     </row>
@@ -1277,13 +2896,16 @@
         <v>1.57</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="25"/>
+      <c r="E28" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.3419999999996</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="29"/>
       <c r="H28" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
     </row>
@@ -1296,13 +2918,16 @@
         <v>1.48</v>
       </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="25"/>
+      <c r="E29" s="10">
+        <f t="shared" si="0"/>
+        <v>2722.4319999999998</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="29"/>
       <c r="H29" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.799999999999997</v>
       </c>
     </row>
@@ -1315,11 +2940,14 @@
         <v>1.42</v>
       </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="15"/>
+      <c r="E30" s="7">
+        <f>$I$5-C30</f>
+        <v>2722.4919999999997</v>
+      </c>
+      <c r="F30" s="13"/>
       <c r="G30" s="1"/>
       <c r="H30" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
     </row>
@@ -1332,13 +2960,16 @@
         <v>1.44</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="15" t="s">
-        <v>50</v>
+      <c r="E31" s="7">
+        <f t="shared" ref="E31:E38" si="2">$I$5-C31</f>
+        <v>2722.4719999999998</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1351,15 +2982,18 @@
         <v>1.425</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="15"/>
+      <c r="E32" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.4869999999996</v>
+      </c>
+      <c r="F32" s="13"/>
       <c r="G32" s="1"/>
       <c r="H32" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>46.5</v>
       </c>
@@ -1368,15 +3002,18 @@
         <v>1.34</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.5719999999997</v>
+      </c>
+      <c r="F33" s="13"/>
       <c r="G33" s="1"/>
       <c r="H33" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>47</v>
       </c>
@@ -1385,15 +3022,18 @@
         <v>1.2949999999999999</v>
       </c>
       <c r="D34" s="7"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="15"/>
+      <c r="E34" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.6169999999997</v>
+      </c>
+      <c r="F34" s="13"/>
       <c r="G34" s="1"/>
       <c r="H34" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>47.5</v>
       </c>
@@ -1402,15 +3042,18 @@
         <v>1.325</v>
       </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="15"/>
+      <c r="E35" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.587</v>
+      </c>
+      <c r="F35" s="13"/>
       <c r="G35" s="1"/>
       <c r="H35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>48</v>
       </c>
@@ -1419,15 +3062,18 @@
         <v>1.325</v>
       </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.587</v>
+      </c>
+      <c r="F36" s="13"/>
       <c r="G36" s="1"/>
       <c r="H36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>48.5</v>
       </c>
@@ -1436,15 +3082,18 @@
         <v>1.36</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.5519999999997</v>
+      </c>
+      <c r="F37" s="13"/>
       <c r="G37" s="1"/>
       <c r="H37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>49</v>
       </c>
@@ -1453,15 +3102,18 @@
         <v>1.333</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="7">
+        <f t="shared" si="2"/>
+        <v>2722.5789999999997</v>
+      </c>
+      <c r="F38" s="13"/>
       <c r="G38" s="1"/>
       <c r="H38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>49.5</v>
       </c>
@@ -1470,17 +3122,20 @@
         <v>1.35</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="15" t="s">
-        <v>54</v>
+      <c r="E39" s="7">
+        <f>$I$5-C39</f>
+        <v>2722.5619999999999</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>50</v>
       </c>
@@ -1491,15 +3146,22 @@
       <c r="D40" s="7">
         <v>1.26</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="15"/>
+      <c r="E40" s="7">
+        <f>$I$5-D40</f>
+        <v>2722.6519999999996</v>
+      </c>
+      <c r="F40" s="13"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="7">
-        <f t="shared" si="0"/>
+      <c r="H40" s="13">
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="22">
+        <f>B40+E40</f>
+        <v>2724.8189999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>50.8</v>
       </c>
@@ -1508,15 +3170,18 @@
         <v>2.165</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="15"/>
+      <c r="E41" s="7">
+        <f>$I$40-C41</f>
+        <v>2722.6539999999995</v>
+      </c>
+      <c r="F41" s="13"/>
       <c r="G41" s="1"/>
       <c r="H41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.299999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>51.1</v>
       </c>
@@ -1525,15 +3190,18 @@
         <v>2.04</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="15"/>
+      <c r="E42" s="7">
+        <f t="shared" ref="E42:E73" si="3">$I$40-C42</f>
+        <v>2722.7789999999995</v>
+      </c>
+      <c r="F42" s="13"/>
       <c r="G42" s="1"/>
       <c r="H42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>51.6</v>
       </c>
@@ -1542,17 +3210,20 @@
         <v>2.12</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="15" t="s">
-        <v>16</v>
+      <c r="E43" s="7">
+        <f t="shared" si="3"/>
+        <v>2722.6989999999996</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>51.8</v>
       </c>
@@ -1561,15 +3232,18 @@
         <v>1.8149999999999999</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="15"/>
+      <c r="E44" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0039999999995</v>
+      </c>
+      <c r="F44" s="13"/>
       <c r="G44" s="1"/>
       <c r="H44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.299999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>52</v>
       </c>
@@ -1578,15 +3252,18 @@
         <v>1.7949999999999999</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="15"/>
+      <c r="E45" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0239999999994</v>
+      </c>
+      <c r="F45" s="13"/>
       <c r="G45" s="1"/>
       <c r="H45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>52.5</v>
       </c>
@@ -1595,15 +3272,18 @@
         <v>1.74</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="15"/>
+      <c r="E46" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0789999999997</v>
+      </c>
+      <c r="F46" s="13"/>
       <c r="G46" s="1"/>
       <c r="H46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>53</v>
       </c>
@@ -1612,15 +3292,18 @@
         <v>1.7450000000000001</v>
       </c>
       <c r="D47" s="7"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0739999999996</v>
+      </c>
+      <c r="F47" s="13"/>
       <c r="G47" s="1"/>
       <c r="H47" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>53.2</v>
       </c>
@@ -1629,17 +3312,30 @@
         <v>1.8149999999999999</v>
       </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="15" t="s">
-        <v>17</v>
+      <c r="E48" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0039999999995</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.700000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="26">
+        <v>2723.14</v>
+      </c>
+      <c r="J48" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K48">
+        <f>I48-E48</f>
+        <v>0.13600000000042201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>53.2</v>
       </c>
@@ -1648,17 +3344,20 @@
         <v>1.72</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="15" t="s">
-        <v>19</v>
+      <c r="E49" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0989999999997</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.700000000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>53.9</v>
       </c>
@@ -1667,17 +3366,20 @@
         <v>1.77</v>
       </c>
       <c r="D50" s="7"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="15" t="s">
-        <v>20</v>
+      <c r="E50" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.0489999999995</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>54.1</v>
       </c>
@@ -1686,17 +3388,20 @@
         <v>1.64</v>
       </c>
       <c r="D51" s="7"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="15" t="s">
-        <v>21</v>
+      <c r="E51" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1789999999996</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.6</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>55.215000000000003</v>
       </c>
@@ -1705,17 +3410,30 @@
         <v>1.63</v>
       </c>
       <c r="D52" s="7"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="15" t="s">
-        <v>49</v>
+      <c r="E52" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1889999999994</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.715000000000003</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="26">
+        <v>2723.3090000000002</v>
+      </c>
+      <c r="J52" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K52">
+        <f>I52-E52</f>
+        <v>0.12000000000080036</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>55.5</v>
       </c>
@@ -1724,17 +3442,20 @@
         <v>1.63</v>
       </c>
       <c r="D53" s="7"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="15" t="s">
-        <v>22</v>
+      <c r="E53" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1889999999994</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>55.5</v>
       </c>
@@ -1743,17 +3464,20 @@
         <v>1.65</v>
       </c>
       <c r="D54" s="7"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="15" t="s">
-        <v>23</v>
+      <c r="E54" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1689999999994</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>56</v>
       </c>
@@ -1762,15 +3486,18 @@
         <v>1.66</v>
       </c>
       <c r="D55" s="7"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="15"/>
+      <c r="E55" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1589999999997</v>
+      </c>
+      <c r="F55" s="13"/>
       <c r="G55" s="1"/>
       <c r="H55" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.5</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>56.5</v>
       </c>
@@ -1779,15 +3506,18 @@
         <v>1.67</v>
       </c>
       <c r="D56" s="7"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="15"/>
+      <c r="E56" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1489999999994</v>
+      </c>
+      <c r="F56" s="13"/>
       <c r="G56" s="1"/>
       <c r="H56" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>57</v>
       </c>
@@ -1796,15 +3526,18 @@
         <v>1.66</v>
       </c>
       <c r="D57" s="7"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="15"/>
+      <c r="E57" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.1589999999997</v>
+      </c>
+      <c r="F57" s="13"/>
       <c r="G57" s="1"/>
       <c r="H57" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>57.5</v>
       </c>
@@ -1813,15 +3546,18 @@
         <v>1.58</v>
       </c>
       <c r="D58" s="7"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="15"/>
+      <c r="E58" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.2389999999996</v>
+      </c>
+      <c r="F58" s="13"/>
       <c r="G58" s="1"/>
       <c r="H58" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -1830,17 +3566,20 @@
         <v>1.56</v>
       </c>
       <c r="D59" s="7"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="15" t="s">
-        <v>24</v>
+      <c r="E59" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.2589999999996</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>58.4</v>
       </c>
@@ -1849,17 +3588,20 @@
         <v>1.3</v>
       </c>
       <c r="D60" s="7"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="15" t="s">
-        <v>25</v>
+      <c r="E60" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.5189999999993</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.9</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>59</v>
       </c>
@@ -1868,17 +3610,30 @@
         <v>1.39</v>
       </c>
       <c r="D61" s="7"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="15" t="s">
-        <v>51</v>
+      <c r="E61" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.4289999999996</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="26">
+        <v>2723.857</v>
+      </c>
+      <c r="J61" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K61">
+        <f>I61-E61</f>
+        <v>0.42800000000033833</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>59.4</v>
       </c>
@@ -1887,17 +3642,21 @@
         <v>1.37</v>
       </c>
       <c r="D62" s="7"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="15" t="s">
-        <v>27</v>
+      <c r="E62" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.4489999999996</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.9</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>59.4</v>
       </c>
@@ -1906,17 +3665,30 @@
         <v>1.4119999999999999</v>
       </c>
       <c r="D63" s="7"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="15" t="s">
-        <v>28</v>
+      <c r="E63" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.4069999999997</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.9</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="26">
+        <v>2723.817</v>
+      </c>
+      <c r="J63" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K63">
+        <f>I63-E63</f>
+        <v>0.41000000000030923</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>60</v>
       </c>
@@ -1925,17 +3697,20 @@
         <v>1.3</v>
       </c>
       <c r="D64" s="7"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="15" t="s">
-        <v>26</v>
+      <c r="E64" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.5189999999993</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>60.3</v>
       </c>
@@ -1944,17 +3719,20 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D65" s="7"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="15" t="s">
-        <v>29</v>
+      <c r="E65" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.6589999999997</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.799999999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>60.5</v>
       </c>
@@ -1963,17 +3741,20 @@
         <v>1.24</v>
       </c>
       <c r="D66" s="7"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="15" t="s">
-        <v>30</v>
+      <c r="E66" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.5789999999997</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>61</v>
       </c>
@@ -1982,17 +3763,20 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="D67" s="7"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="15" t="s">
-        <v>31</v>
+      <c r="E67" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.7089999999994</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>61.5</v>
       </c>
@@ -2001,17 +3785,20 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="D68" s="7"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="15" t="s">
-        <v>31</v>
+      <c r="E68" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.6689999999994</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>62</v>
       </c>
@@ -2020,34 +3807,40 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="D69" s="7"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="15" t="s">
-        <v>32</v>
+      <c r="E69" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.7089999999994</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.5</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>62.5</v>
       </c>
       <c r="B70" s="7"/>
-      <c r="C70" s="7" t="s">
-        <v>18</v>
+      <c r="C70" s="7">
+        <v>1</v>
       </c>
       <c r="D70" s="7"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="15"/>
+      <c r="E70" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.8189999999995</v>
+      </c>
+      <c r="F70" s="13"/>
       <c r="G70" s="1"/>
       <c r="H70" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>63</v>
       </c>
@@ -2056,15 +3849,18 @@
         <v>0.98</v>
       </c>
       <c r="D71" s="7"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="15"/>
+      <c r="E71" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.8389999999995</v>
+      </c>
+      <c r="F71" s="13"/>
       <c r="G71" s="1"/>
       <c r="H71" s="7">
-        <f t="shared" ref="H71:H96" si="1">A71-32.5</f>
+        <f t="shared" ref="H71:H96" si="4">A71-32.5</f>
         <v>30.5</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>63.5</v>
       </c>
@@ -2073,17 +3869,30 @@
         <v>0.98</v>
       </c>
       <c r="D72" s="7"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="15" t="s">
-        <v>33</v>
+      <c r="E72" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.8389999999995</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="G72" s="1"/>
       <c r="H72" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="26">
+        <v>2724.3589999999999</v>
+      </c>
+      <c r="J72" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K72">
+        <f>I72-E72</f>
+        <v>0.52000000000043656</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>64</v>
       </c>
@@ -2092,17 +3901,20 @@
         <v>0.94</v>
       </c>
       <c r="D73" s="7"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="15" t="s">
-        <v>34</v>
+      <c r="E73" s="7">
+        <f t="shared" si="3"/>
+        <v>2723.8789999999995</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="G73" s="1"/>
       <c r="H73" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>31.5</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>64.5</v>
       </c>
@@ -2111,15 +3923,18 @@
         <v>0.89500000000000002</v>
       </c>
       <c r="D74" s="7"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="15"/>
+      <c r="E74" s="7">
+        <f>$I$40-C74</f>
+        <v>2723.9239999999995</v>
+      </c>
+      <c r="F74" s="13"/>
       <c r="G74" s="1"/>
       <c r="H74" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>65</v>
       </c>
@@ -2130,108 +3945,140 @@
       <c r="D75" s="7">
         <v>0.93500000000000005</v>
       </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="15" t="s">
-        <v>26</v>
+      <c r="E75" s="7">
+        <f>$I$40-D75</f>
+        <v>2723.8839999999996</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="G75" s="1"/>
-      <c r="H75" s="7">
-        <f t="shared" si="1"/>
+      <c r="H75" s="13">
+        <f t="shared" si="4"/>
         <v>32.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="16">
+      <c r="I75" s="22">
+        <f>B75+E75</f>
+        <v>2727.0639999999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
         <v>65.7</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16">
+      <c r="B76" s="14"/>
+      <c r="C76" s="14">
         <v>2.9849999999999999</v>
       </c>
-      <c r="D76" s="16"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G76" s="26" t="s">
-        <v>37</v>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14">
+        <f>$I$75-C76</f>
+        <v>2724.0789999999993</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G76" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="H76" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="16">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
         <v>66</v>
       </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14">
         <v>2.9</v>
       </c>
-      <c r="D77" s="16"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="26"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14">
+        <f t="shared" ref="E77:E80" si="5">$I$75-C77</f>
+        <v>2724.1639999999993</v>
+      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="30"/>
       <c r="H77" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>33.5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="16">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
         <v>66.5</v>
       </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16">
+      <c r="B78" s="14"/>
+      <c r="C78" s="14">
         <v>2.88</v>
       </c>
-      <c r="D78" s="16"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="26"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14">
+        <f t="shared" si="5"/>
+        <v>2724.1839999999993</v>
+      </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="30"/>
       <c r="H78" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="16">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
         <v>67</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16">
+      <c r="B79" s="14"/>
+      <c r="C79" s="14">
         <v>2.85</v>
       </c>
-      <c r="D79" s="16"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="18" t="s">
+      <c r="D79" s="14"/>
+      <c r="E79" s="14">
+        <f t="shared" si="5"/>
+        <v>2724.2139999999995</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G79" s="30"/>
+      <c r="H79" s="7">
+        <f t="shared" si="4"/>
+        <v>34.5</v>
+      </c>
+      <c r="I79" s="26">
+        <v>2724.1610000000001</v>
+      </c>
+      <c r="J79" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K79">
+        <f>I79-E79</f>
+        <v>-5.2999999999428837E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <v>67.5</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14">
+        <v>2.87</v>
+      </c>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14">
+        <f t="shared" si="5"/>
+        <v>2724.1939999999995</v>
+      </c>
+      <c r="F80" s="15"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="7">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="G79" s="26"/>
-      <c r="H79" s="7">
-        <f t="shared" si="1"/>
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="16">
-        <v>67.5</v>
-      </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16">
-        <v>2.87</v>
-      </c>
-      <c r="D80" s="16"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="7">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>67.8</v>
       </c>
@@ -2240,17 +4087,20 @@
         <v>2.835</v>
       </c>
       <c r="D81" s="7"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="15" t="s">
-        <v>26</v>
+      <c r="E81" s="7">
+        <f>$I$75-C81</f>
+        <v>2724.2289999999994</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="G81" s="1"/>
       <c r="H81" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>67.900000000000006</v>
       </c>
@@ -2259,17 +4109,20 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="D82" s="7"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="15" t="s">
-        <v>36</v>
+      <c r="E82" s="7">
+        <f t="shared" ref="E82:E97" si="6">$I$75-C82</f>
+        <v>2724.5539999999992</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35.400000000000006</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>68.2</v>
       </c>
@@ -2278,17 +4131,20 @@
         <v>2.44</v>
       </c>
       <c r="D83" s="7"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="15" t="s">
-        <v>25</v>
+      <c r="E83" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.6239999999993</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="G83" s="1"/>
       <c r="H83" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>68.7</v>
       </c>
@@ -2297,15 +4153,18 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="D84" s="7"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="15"/>
+      <c r="E84" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.5539999999992</v>
+      </c>
+      <c r="F84" s="13"/>
       <c r="G84" s="1"/>
       <c r="H84" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>69</v>
       </c>
@@ -2314,15 +4173,18 @@
         <v>2.48</v>
       </c>
       <c r="D85" s="7"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="15"/>
+      <c r="E85" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.5839999999994</v>
+      </c>
+      <c r="F85" s="13"/>
       <c r="G85" s="1"/>
       <c r="H85" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36.5</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>69.400000000000006</v>
       </c>
@@ -2331,17 +4193,20 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="D86" s="7"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="15" t="s">
-        <v>38</v>
+      <c r="E86" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.5539999999992</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>36.900000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>69.7</v>
       </c>
@@ -2350,17 +4215,20 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="D87" s="7"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="15" t="s">
-        <v>38</v>
+      <c r="E87" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.5739999999996</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>70</v>
       </c>
@@ -2369,17 +4237,20 @@
         <v>2.46</v>
       </c>
       <c r="D88" s="7"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="15" t="s">
-        <v>39</v>
+      <c r="E88" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.6039999999994</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>70.5</v>
       </c>
@@ -2388,17 +4259,20 @@
         <v>2.4249999999999998</v>
       </c>
       <c r="D89" s="7"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="15" t="s">
-        <v>46</v>
+      <c r="E89" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.6389999999992</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>71</v>
       </c>
@@ -2407,55 +4281,71 @@
         <v>2.4049999999999998</v>
       </c>
       <c r="D90" s="7"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="15"/>
+      <c r="E90" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.6589999999992</v>
+      </c>
+      <c r="F90" s="13"/>
       <c r="G90" s="1"/>
       <c r="H90" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38.5</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="19">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="16">
         <v>71.5</v>
       </c>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19">
+      <c r="B91" s="16"/>
+      <c r="C91" s="16">
         <v>2.42</v>
       </c>
-      <c r="D91" s="19"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G91" s="27" t="s">
-        <v>43</v>
+      <c r="D91" s="16"/>
+      <c r="E91" s="16">
+        <f t="shared" si="6"/>
+        <v>2724.6439999999993</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G91" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="H91" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="19">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="16">
         <v>72</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19">
+      <c r="B92" s="16"/>
+      <c r="C92" s="16">
         <v>2.4049999999999998</v>
       </c>
-      <c r="D92" s="19"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="G92" s="27"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16">
+        <f t="shared" si="6"/>
+        <v>2724.6589999999992</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92" s="31"/>
       <c r="H92" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="26">
+        <v>2724.8220000000001</v>
+      </c>
+      <c r="K92">
+        <f>I92-E92</f>
+        <v>0.16300000000092041</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>72.2</v>
       </c>
@@ -2464,15 +4354,18 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="D93" s="7"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="15"/>
+      <c r="E93" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.7439999999992</v>
+      </c>
+      <c r="F93" s="13"/>
       <c r="G93" s="1"/>
       <c r="H93" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>72.5</v>
       </c>
@@ -2481,15 +4374,18 @@
         <v>2.3149999999999999</v>
       </c>
       <c r="D94" s="7"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="15"/>
+      <c r="E94" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.7489999999993</v>
+      </c>
+      <c r="F94" s="13"/>
       <c r="G94" s="1"/>
       <c r="H94" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>73</v>
       </c>
@@ -2498,15 +4394,18 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="D95" s="7"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="15"/>
+      <c r="E95" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.7439999999992</v>
+      </c>
+      <c r="F95" s="13"/>
       <c r="G95" s="1"/>
       <c r="H95" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40.5</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>73.5</v>
       </c>
@@ -2515,13 +4414,16 @@
         <v>2.35</v>
       </c>
       <c r="D96" s="7"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="15" t="s">
-        <v>42</v>
+      <c r="E96" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.7139999999995</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="G96" s="1"/>
       <c r="H96" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
     </row>
@@ -2534,8 +4436,11 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="D97" s="7"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="15"/>
+      <c r="E97" s="7">
+        <f t="shared" si="6"/>
+        <v>2724.7439999999992</v>
+      </c>
+      <c r="F97" s="13"/>
       <c r="G97" s="1"/>
       <c r="H97" s="7">
         <f>A97-32.5</f>
@@ -2550,5 +4455,6 @@
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avg hyporheic analytical and MLEn for T2 ant T3
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
+++ b/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B11AD-EEF6-4A15-852E-70B0FA0F75B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFCFCA8-BCC3-4C5D-9DD0-638627616307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -638,7 +638,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1298,7 +1298,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1853073408"/>
@@ -1360,7 +1360,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1853070912"/>
@@ -1408,7 +1408,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2315,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64046064-0207-40E0-86BF-2B34A938C764}">
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
-        <f t="shared" si="0"/>
+        <f>$I$5-C9</f>
         <v>2721.732</v>
       </c>
       <c r="F9" s="12"/>

</xml_diff>

<commit_message>
estoy dejando la zorra papi
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
+++ b/Topography/LaJara_TopoSurvey/DownReach_LongProfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFCFCA8-BCC3-4C5D-9DD0-638627616307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AD7CC7-53D5-4F7F-95E4-E3E4821AEC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
   </bookViews>
@@ -209,7 +209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +225,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -497,6 +509,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2315,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64046064-0207-40E0-86BF-2B34A938C764}">
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,11 +3145,11 @@
         <f>$I$5-C39</f>
         <v>2722.5619999999999</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="7">
+      <c r="G39" s="33"/>
+      <c r="H39" s="34">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -3150,9 +3169,9 @@
         <f>$I$5-D40</f>
         <v>2722.6519999999996</v>
       </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="13">
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="32">
         <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
@@ -3174,9 +3193,9 @@
         <f>$I$40-C41</f>
         <v>2722.6539999999995</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="7">
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="34">
         <f t="shared" si="1"/>
         <v>18.299999999999997</v>
       </c>
@@ -3194,9 +3213,9 @@
         <f t="shared" ref="E42:E73" si="3">$I$40-C42</f>
         <v>2722.7789999999995</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="7">
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="34">
         <f t="shared" si="1"/>
         <v>18.600000000000001</v>
       </c>
@@ -3214,11 +3233,11 @@
         <f t="shared" si="3"/>
         <v>2722.6989999999996</v>
       </c>
-      <c r="F43" s="13" t="s">
+      <c r="F43" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="7">
+      <c r="G43" s="33"/>
+      <c r="H43" s="34">
         <f t="shared" si="1"/>
         <v>19.100000000000001</v>
       </c>
@@ -3236,9 +3255,9 @@
         <f t="shared" si="3"/>
         <v>2723.0039999999995</v>
       </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="7">
+      <c r="F44" s="32"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="34">
         <f t="shared" si="1"/>
         <v>19.299999999999997</v>
       </c>
@@ -3256,9 +3275,9 @@
         <f t="shared" si="3"/>
         <v>2723.0239999999994</v>
       </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="7">
+      <c r="F45" s="32"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="34">
         <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
@@ -3276,9 +3295,9 @@
         <f t="shared" si="3"/>
         <v>2723.0789999999997</v>
       </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="7">
+      <c r="F46" s="32"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="34">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -3296,9 +3315,9 @@
         <f t="shared" si="3"/>
         <v>2723.0739999999996</v>
       </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="7">
+      <c r="F47" s="32"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34">
         <f t="shared" si="1"/>
         <v>20.5</v>
       </c>
@@ -3316,11 +3335,11 @@
         <f t="shared" si="3"/>
         <v>2723.0039999999995</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="7">
+      <c r="G48" s="33"/>
+      <c r="H48" s="34">
         <f t="shared" si="1"/>
         <v>20.700000000000003</v>
       </c>
@@ -3348,11 +3367,11 @@
         <f t="shared" si="3"/>
         <v>2723.0989999999997</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="7">
+      <c r="G49" s="33"/>
+      <c r="H49" s="34">
         <f t="shared" si="1"/>
         <v>20.700000000000003</v>
       </c>
@@ -3370,11 +3389,11 @@
         <f t="shared" si="3"/>
         <v>2723.0489999999995</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F50" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="7">
+      <c r="G50" s="33"/>
+      <c r="H50" s="34">
         <f t="shared" si="1"/>
         <v>21.4</v>
       </c>
@@ -3392,11 +3411,11 @@
         <f t="shared" si="3"/>
         <v>2723.1789999999996</v>
       </c>
-      <c r="F51" s="13" t="s">
+      <c r="F51" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="7">
+      <c r="G51" s="33"/>
+      <c r="H51" s="34">
         <f t="shared" si="1"/>
         <v>21.6</v>
       </c>
@@ -3414,11 +3433,11 @@
         <f t="shared" si="3"/>
         <v>2723.1889999999994</v>
       </c>
-      <c r="F52" s="13" t="s">
+      <c r="F52" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="7">
+      <c r="G52" s="33"/>
+      <c r="H52" s="34">
         <f t="shared" si="1"/>
         <v>22.715000000000003</v>
       </c>
@@ -3446,11 +3465,11 @@
         <f t="shared" si="3"/>
         <v>2723.1889999999994</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="7">
+      <c r="G53" s="33"/>
+      <c r="H53" s="34">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>

</xml_diff>